<commit_message>
added eem sync diagram
</commit_message>
<xml_diff>
--- a/written-blueprint-checklist.xlsx
+++ b/written-blueprint-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qdd/Google Drive/git/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA99A49A-DD80-1C45-BD84-21717C369228}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3B9550-41B4-B048-A501-B9535C4A4445}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-74220" yWindow="700" windowWidth="26220" windowHeight="18780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="topics" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="651">
   <si>
     <t>3-node architecture</t>
   </si>
@@ -2613,27 +2613,12 @@
     <t>buckets and colors</t>
   </si>
   <si>
-    <t>version differences</t>
-  </si>
-  <si>
-    <t>schedule, life commands</t>
-  </si>
-  <si>
-    <t>how it works, end-to-end reachability, transport headers, state, diff nat66</t>
-  </si>
-  <si>
     <t>NAT-PT</t>
   </si>
   <si>
     <t>nx-api, securing, cisco virtual topology</t>
   </si>
   <si>
-    <t>encapsulation</t>
-  </si>
-  <si>
-    <t>options</t>
-  </si>
-  <si>
     <t>address composition</t>
   </si>
   <si>
@@ -2650,15 +2635,6 @@
   </si>
   <si>
     <t>regexp practice</t>
-  </si>
-  <si>
-    <t>ntp commands, version differences</t>
-  </si>
-  <si>
-    <t>review examples</t>
-  </si>
-  <si>
-    <t>review different components</t>
   </si>
   <si>
     <t>review cisco product functionality</t>
@@ -3761,8 +3737,8 @@
   <dimension ref="A1:I892"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A346" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D109" sqref="D109"/>
+      <pane ySplit="1" topLeftCell="A400" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A424" sqref="A424"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3786,10 +3762,10 @@
         <v>4</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>621</v>
@@ -3799,7 +3775,7 @@
       </c>
       <c r="G1" s="13">
         <f ca="1">(TODAY()-I1)*-1</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H1" s="16" t="s">
         <v>22</v>
@@ -4610,10 +4586,10 @@
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E55" s="87" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="F55" s="9"/>
       <c r="G55" s="14"/>
@@ -4987,10 +4963,10 @@
       </c>
       <c r="C80" s="86"/>
       <c r="D80" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E80" s="90" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="F80" s="9"/>
       <c r="G80" s="14"/>
@@ -5426,7 +5402,7 @@
       </c>
       <c r="C109" s="8"/>
       <c r="D109" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E109" s="87" t="s">
         <v>622</v>
@@ -5818,7 +5794,7 @@
       </c>
       <c r="C135" s="8"/>
       <c r="D135" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E135" s="87"/>
       <c r="F135" s="9"/>
@@ -6105,10 +6081,10 @@
       </c>
       <c r="C154" s="8"/>
       <c r="D154" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E154" s="89" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
       <c r="F154" s="9"/>
       <c r="G154" s="14"/>
@@ -6469,10 +6445,10 @@
       </c>
       <c r="C178" s="8"/>
       <c r="D178" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E178" s="87" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="F178" s="9"/>
       <c r="G178" s="14"/>
@@ -6638,10 +6614,10 @@
       </c>
       <c r="C189" s="8"/>
       <c r="D189" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E189" s="89" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
       <c r="F189" s="9"/>
       <c r="G189" s="14"/>
@@ -6972,10 +6948,10 @@
       </c>
       <c r="C211" s="8"/>
       <c r="D211" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E211" s="87" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="F211" s="9"/>
       <c r="G211" s="14"/>
@@ -7275,10 +7251,10 @@
       </c>
       <c r="C231" s="8"/>
       <c r="D231" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E231" s="90" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="F231" s="9"/>
       <c r="G231" s="14"/>
@@ -7294,10 +7270,10 @@
       </c>
       <c r="C232" s="8"/>
       <c r="D232" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E232" s="90" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="F232" s="9"/>
       <c r="G232" s="14"/>
@@ -7523,10 +7499,10 @@
       </c>
       <c r="C247" s="8"/>
       <c r="D247" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E247" s="89" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
       <c r="F247" s="9"/>
       <c r="G247" s="14"/>
@@ -7542,10 +7518,10 @@
       </c>
       <c r="C248" s="8"/>
       <c r="D248" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E248" s="87" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="F248" s="9"/>
       <c r="G248" s="14"/>
@@ -7561,10 +7537,10 @@
       </c>
       <c r="C249" s="8"/>
       <c r="D249" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E249" s="90" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
       <c r="F249" s="9"/>
       <c r="G249" s="14"/>
@@ -7730,10 +7706,10 @@
       </c>
       <c r="C260" s="8"/>
       <c r="D260" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E260" s="87" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="F260" s="9"/>
       <c r="G260" s="14"/>
@@ -7764,10 +7740,10 @@
       </c>
       <c r="C262" s="8"/>
       <c r="D262" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E262" s="87" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="F262" s="9"/>
       <c r="G262" s="14"/>
@@ -7843,10 +7819,10 @@
       </c>
       <c r="C267" s="8"/>
       <c r="D267" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E267" s="89" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="F267" s="9"/>
       <c r="G267" s="14"/>
@@ -7952,10 +7928,10 @@
       </c>
       <c r="C274" s="8"/>
       <c r="D274" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E274" s="87" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="F274" s="9"/>
       <c r="G274" s="14"/>
@@ -8269,10 +8245,10 @@
       </c>
       <c r="C295" s="8"/>
       <c r="D295" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E295" s="90" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
       <c r="F295" s="9"/>
       <c r="G295" s="14"/>
@@ -8288,10 +8264,10 @@
       </c>
       <c r="C296" s="8"/>
       <c r="D296" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E296" s="87" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="F296" s="9"/>
       <c r="G296" s="14"/>
@@ -8322,10 +8298,10 @@
       </c>
       <c r="C298" s="8"/>
       <c r="D298" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E298" s="87" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
       <c r="F298" s="9"/>
       <c r="G298" s="14"/>
@@ -8416,10 +8392,10 @@
       </c>
       <c r="C304" s="8"/>
       <c r="D304" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E304" s="90" t="s">
-        <v>654</v>
+        <v>646</v>
       </c>
       <c r="F304" s="9"/>
       <c r="G304" s="14"/>
@@ -8465,7 +8441,7 @@
       </c>
       <c r="C307" s="8"/>
       <c r="D307" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E307" s="87"/>
       <c r="F307" s="9"/>
@@ -8497,10 +8473,10 @@
       </c>
       <c r="C309" s="8"/>
       <c r="D309" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E309" s="90" t="s">
-        <v>655</v>
+        <v>647</v>
       </c>
       <c r="F309" s="9"/>
       <c r="G309" s="14"/>
@@ -8724,10 +8700,10 @@
       </c>
       <c r="C324" s="8"/>
       <c r="D324" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="E324" s="90" t="s">
         <v>648</v>
-      </c>
-      <c r="E324" s="90" t="s">
-        <v>656</v>
       </c>
       <c r="F324" s="9"/>
       <c r="G324" s="14"/>
@@ -8818,10 +8794,10 @@
       </c>
       <c r="C330" s="8"/>
       <c r="D330" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E330" s="90" t="s">
-        <v>657</v>
+        <v>649</v>
       </c>
       <c r="F330" s="9"/>
       <c r="G330" s="14"/>
@@ -9046,7 +9022,7 @@
         <v>387</v>
       </c>
       <c r="C345" s="8" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="D345" s="9"/>
       <c r="E345" s="87" t="s">
@@ -9110,7 +9086,7 @@
         <v>391</v>
       </c>
       <c r="C349" s="8" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="D349" s="9"/>
       <c r="E349" s="87"/>
@@ -9396,7 +9372,7 @@
       </c>
       <c r="C368" s="8"/>
       <c r="D368" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E368" s="87" t="s">
         <v>624</v>
@@ -9426,9 +9402,7 @@
       <c r="B370" s="8" t="s">
         <v>413</v>
       </c>
-      <c r="C370" s="8" t="s">
-        <v>648</v>
-      </c>
+      <c r="C370" s="8"/>
       <c r="D370" s="9"/>
       <c r="E370" s="87"/>
       <c r="F370" s="9"/>
@@ -9475,10 +9449,10 @@
       </c>
       <c r="C373" s="8"/>
       <c r="D373" s="9" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="E373" s="90" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
       <c r="F373" s="9"/>
       <c r="G373" s="14"/>
@@ -9582,13 +9556,9 @@
       <c r="B380" s="8" t="s">
         <v>423</v>
       </c>
-      <c r="C380" s="8" t="s">
-        <v>648</v>
-      </c>
+      <c r="C380" s="8"/>
       <c r="D380" s="9"/>
-      <c r="E380" s="87" t="s">
-        <v>638</v>
-      </c>
+      <c r="E380" s="87"/>
       <c r="F380" s="9"/>
       <c r="G380" s="14"/>
       <c r="H380" s="14"/>
@@ -9601,9 +9571,7 @@
       <c r="B381" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="C381" s="8" t="s">
-        <v>648</v>
-      </c>
+      <c r="C381" s="8"/>
       <c r="D381" s="9"/>
       <c r="E381" s="87"/>
       <c r="F381" s="9"/>
@@ -9678,9 +9646,7 @@
       <c r="B386" s="8" t="s">
         <v>429</v>
       </c>
-      <c r="C386" s="8" t="s">
-        <v>648</v>
-      </c>
+      <c r="C386" s="8"/>
       <c r="D386" s="9"/>
       <c r="E386" s="87"/>
       <c r="F386" s="9"/>
@@ -9695,9 +9661,7 @@
       <c r="B387" s="8" t="s">
         <v>430</v>
       </c>
-      <c r="C387" s="8" t="s">
-        <v>648</v>
-      </c>
+      <c r="C387" s="8"/>
       <c r="D387" s="9"/>
       <c r="E387" s="87"/>
       <c r="F387" s="9"/>
@@ -9712,9 +9676,7 @@
       <c r="B388" s="8" t="s">
         <v>431</v>
       </c>
-      <c r="C388" s="8" t="s">
-        <v>648</v>
-      </c>
+      <c r="C388" s="8"/>
       <c r="D388" s="9"/>
       <c r="E388" s="87"/>
       <c r="F388" s="9"/>
@@ -9744,12 +9706,12 @@
       <c r="B390" s="8" t="s">
         <v>433</v>
       </c>
-      <c r="C390" s="8" t="s">
-        <v>648</v>
-      </c>
-      <c r="D390" s="9"/>
+      <c r="C390" s="8"/>
+      <c r="D390" s="9" t="s">
+        <v>640</v>
+      </c>
       <c r="E390" s="87" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="F390" s="9"/>
       <c r="G390" s="14"/>
@@ -9793,13 +9755,9 @@
       <c r="B393" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="C393" s="8" t="s">
-        <v>648</v>
-      </c>
+      <c r="C393" s="8"/>
       <c r="D393" s="9"/>
-      <c r="E393" s="87" t="s">
-        <v>630</v>
-      </c>
+      <c r="E393" s="87"/>
       <c r="F393" s="9"/>
       <c r="G393" s="14"/>
       <c r="H393" s="14"/>
@@ -9812,13 +9770,9 @@
       <c r="B394" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="C394" s="9" t="s">
-        <v>648</v>
-      </c>
+      <c r="C394" s="9"/>
       <c r="D394" s="9"/>
-      <c r="E394" s="87" t="s">
-        <v>627</v>
-      </c>
+      <c r="E394" s="87"/>
       <c r="F394" s="9"/>
       <c r="G394" s="14"/>
       <c r="H394" s="14"/>
@@ -9846,13 +9800,9 @@
       <c r="B396" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="C396" s="8" t="s">
-        <v>648</v>
-      </c>
+      <c r="C396" s="8"/>
       <c r="D396" s="9"/>
-      <c r="E396" s="87" t="s">
-        <v>626</v>
-      </c>
+      <c r="E396" s="87"/>
       <c r="F396" s="9"/>
       <c r="G396" s="14"/>
       <c r="H396" s="14"/>
@@ -9865,9 +9815,7 @@
       <c r="B397" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="C397" s="8" t="s">
-        <v>648</v>
-      </c>
+      <c r="C397" s="8"/>
       <c r="D397" s="9"/>
       <c r="E397" s="87"/>
       <c r="G397" s="14"/>
@@ -9941,13 +9889,9 @@
       <c r="B402" s="8" t="s">
         <v>445</v>
       </c>
-      <c r="C402" s="8" t="s">
-        <v>648</v>
-      </c>
+      <c r="C402" s="8"/>
       <c r="D402" s="9"/>
-      <c r="E402" s="87" t="s">
-        <v>625</v>
-      </c>
+      <c r="E402" s="87"/>
       <c r="F402" s="9"/>
       <c r="G402" s="14"/>
       <c r="H402" s="14"/>
@@ -9975,13 +9919,9 @@
       <c r="B404" s="8" t="s">
         <v>447</v>
       </c>
-      <c r="C404" s="8" t="s">
-        <v>648</v>
-      </c>
+      <c r="C404" s="8"/>
       <c r="D404" s="9"/>
-      <c r="E404" s="87" t="s">
-        <v>631</v>
-      </c>
+      <c r="E404" s="87"/>
       <c r="F404" s="9"/>
       <c r="G404" s="14"/>
       <c r="H404" s="14"/>
@@ -10009,13 +9949,9 @@
       <c r="B406" s="8" t="s">
         <v>449</v>
       </c>
-      <c r="C406" s="8" t="s">
-        <v>648</v>
-      </c>
+      <c r="C406" s="8"/>
       <c r="D406" s="9"/>
-      <c r="E406" s="87" t="s">
-        <v>639</v>
-      </c>
+      <c r="E406" s="87"/>
       <c r="F406" s="9"/>
       <c r="G406" s="14"/>
       <c r="H406" s="14"/>
@@ -10221,13 +10157,9 @@
       <c r="B420" s="8" t="s">
         <v>464</v>
       </c>
-      <c r="C420" s="8" t="s">
-        <v>648</v>
-      </c>
+      <c r="C420" s="8"/>
       <c r="D420" s="9"/>
-      <c r="E420" s="87" t="s">
-        <v>640</v>
-      </c>
+      <c r="E420" s="87"/>
       <c r="F420" s="9"/>
       <c r="G420" s="14"/>
       <c r="H420" s="14"/>
@@ -10240,12 +10172,12 @@
       <c r="B421" s="8" t="s">
         <v>465</v>
       </c>
-      <c r="C421" s="8" t="s">
-        <v>648</v>
-      </c>
-      <c r="D421" s="9"/>
+      <c r="C421" s="8"/>
+      <c r="D421" s="9" t="s">
+        <v>640</v>
+      </c>
       <c r="E421" s="87" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
       <c r="F421" s="9"/>
       <c r="G421" s="14"/>
@@ -10319,12 +10251,12 @@
       <c r="B426" s="8" t="s">
         <v>470</v>
       </c>
-      <c r="C426" s="8" t="s">
-        <v>648</v>
-      </c>
-      <c r="D426" s="9"/>
+      <c r="C426" s="8"/>
+      <c r="D426" s="9" t="s">
+        <v>640</v>
+      </c>
       <c r="E426" s="87" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="F426" s="9"/>
       <c r="G426" s="14"/>
@@ -10339,11 +10271,11 @@
         <v>471</v>
       </c>
       <c r="C427" s="8" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="D427" s="9"/>
       <c r="E427" s="87" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
       <c r="F427" s="9"/>
       <c r="G427" s="14"/>

</xml_diff>